<commit_message>
Bring onboarding templates up to date
- Adds automated assessment framework V1 CSV template
- Deletes unused self assessment framework CSV templates
- Updates contents of YAML, XLSX and CSV templates
</commit_message>
<xml_diff>
--- a/AWSVendorInsightsSecuritySelfAssessment_2022-11-30.xlsx
+++ b/AWSVendorInsightsSecuritySelfAssessment_2022-11-30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adittyim/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jianfeim/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07EFE10-73A2-B74A-BB1E-0E8762700D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473AD042-B183-5A4F-A085-FC03B27008B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34920" yWindow="-4140" windowWidth="37580" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30720" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -1363,9 +1363,6 @@
     <t>List any additional certificates that are currently being audited or reviewed with an estimated completion date.</t>
   </si>
   <si>
-    <t>Specify if formal procedures are developed and maintained for business continuity. If yes, provide more details D52on the procedures.</t>
-  </si>
-  <si>
     <t>control-ad8wlrnw</t>
   </si>
   <si>
@@ -1541,6 +1538,9 @@
   </si>
   <si>
     <t>Detailed Response</t>
+  </si>
+  <si>
+    <t>Specify if formal procedures are developed and maintained for business continuity. If yes, provide more details on the procedures.</t>
   </si>
 </sst>
 </file>
@@ -1934,15 +1934,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="50.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="51" style="4" customWidth="1"/>
     <col min="4" max="4" width="70.83203125" style="4" customWidth="1"/>
@@ -1976,10 +1976,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>504</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2640,7 +2640,7 @@
     </row>
     <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>146</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="45" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>149</v>
@@ -2672,7 +2672,7 @@
     </row>
     <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>152</v>
@@ -2688,7 +2688,7 @@
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>155</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>158</v>
@@ -2720,7 +2720,7 @@
     </row>
     <row r="49" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>161</v>
@@ -2761,7 +2761,7 @@
         <v>170</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>446</v>
+        <v>505</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2793,14 +2793,14 @@
         <v>177</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>178</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="55" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>181</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="56" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>184</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="57" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>187</v>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="58" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>190</v>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="59" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>193</v>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="60" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>196</v>
@@ -2905,14 +2905,14 @@
         <v>197</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>198</v>
@@ -2921,14 +2921,14 @@
         <v>199</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>200</v>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="63" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>203</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>206</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="65" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>209</v>
@@ -3033,14 +3033,14 @@
         <v>222</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>223</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="70" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>226</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="71" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>229</v>
@@ -3088,7 +3088,7 @@
     </row>
     <row r="72" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>232</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="73" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>235</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="74" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>238</v>
@@ -3136,7 +3136,7 @@
     </row>
     <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>241</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="76" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>244</v>
@@ -3168,23 +3168,23 @@
     </row>
     <row r="77" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="D77" s="4" t="s">
         <v>479</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>480</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>247</v>
@@ -3193,7 +3193,7 @@
         <v>248</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
@@ -3264,7 +3264,7 @@
     </row>
     <row r="83" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>265</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="85" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>272</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="87" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>279</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="89" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>286</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="90" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>289</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="95" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>308</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="99" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>323</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="100" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>326</v>
@@ -3616,16 +3616,16 @@
     </row>
     <row r="105" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="C105" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="C105" s="4" t="s">
+      <c r="D105" s="4" t="s">
         <v>493</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>494</v>
       </c>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="109" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>357</v>
@@ -3712,7 +3712,7 @@
     </row>
     <row r="111" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>364</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="112" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>367</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="114" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>374</v>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="117" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>385</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="118" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>388</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="122" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>403</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="125" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>413</v>
@@ -3952,7 +3952,7 @@
     </row>
     <row r="126" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>416</v>
@@ -3983,12 +3983,12 @@
       <c r="F127" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mGX52oxFkL0fDci6h7ldR8FohVrTrAVft36C9H9GmgIKVk0A9axAzpN4E8tNSMxiIMj0EXGoIy9MK1Ml3MEciQ==" saltValue="zKwVy6s0nfECl6x5flRU0g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="g7wZIVewBraFDN6Ss/FTiOJLJ7goD+kZkQ7RU/MYw7nKC2v0OQWmD/U5/uMzwUJozHMlbpBrq6sXquiXp0iesA==" saltValue="5/rYC+7kcUZeatytj9H8Aw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E3:E5 E106:E127 E62:E66 E42:E59 E68 E79:E86 E88:E104 E67 E7:E39 E87 E69:E72 E74:E77" xr:uid="{33984C94-1769-7949-8D41-660A366B8F89}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E62:E76 E42:E59 E3:E39 E79:E104 E106:E121 E123:E127" xr:uid="{33984C94-1769-7949-8D41-660A366B8F89}">
       <formula1>"N/A., Yes., No."</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>